<commit_message>
new sim results and new calculation
</commit_message>
<xml_diff>
--- a/out_of_sample_direct_results/dunn_matrix_equalw_out_sample_direct_t126.xlsx
+++ b/out_of_sample_direct_results/dunn_matrix_equalw_out_sample_direct_t126.xlsx
@@ -10,14 +10,15 @@
     <sheet name="annualised_return" sheetId="1" r:id="rId1"/>
     <sheet name="mean_period_return" sheetId="2" r:id="rId2"/>
     <sheet name="sharpe_annualized" sheetId="3" r:id="rId3"/>
-    <sheet name="VaR" sheetId="4" r:id="rId4"/>
+    <sheet name="sharpe_period" sheetId="4" r:id="rId4"/>
+    <sheet name="VaR" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="10">
   <si>
     <t>minvar_ports_equalw</t>
   </si>
@@ -459,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.0106</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -494,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.0003</v>
+        <v>0.0325</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -587,10 +588,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.0106</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0.0003</v>
+        <v>0.0325</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -640,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.0004</v>
+        <v>0.0183</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -649,7 +650,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0.5657</v>
+        <v>0.0023</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -672,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.0004</v>
+        <v>0.0183</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -716,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.0019</v>
+        <v>0.0131</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -748,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.0019</v>
+        <v>0.0131</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -777,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.5657</v>
+        <v>0.0023</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -854,7 +855,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.0106</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -889,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.0003</v>
+        <v>0.0325</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -982,10 +983,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.0106</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0.0003</v>
+        <v>0.0325</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1035,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.0004</v>
+        <v>0.0183</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1044,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0.5657</v>
+        <v>0.0023</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1067,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.0004</v>
+        <v>0.0183</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1111,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.0019</v>
+        <v>0.0131</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1143,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.0019</v>
+        <v>0.0131</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1172,7 +1173,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.5657</v>
+        <v>0.0023</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1252,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1281,10 +1282,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="F3">
-        <v>0.1727</v>
+        <v>0.3847</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1319,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1334,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0.0071</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1345,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1354,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1369,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0.0068</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1380,13 +1381,13 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.1727</v>
+        <v>0.3847</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1412,7 +1413,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1430,10 +1431,10 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1462,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1471,10 +1472,10 @@
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.0018</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1497,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1506,10 +1507,10 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.0007</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>0.0011</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1535,10 +1536,10 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.0018</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.0007</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1558,10 +1559,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0.0071</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.0068</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1570,10 +1571,10 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>0.0004</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.0011</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1647,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1673,13 +1674,13 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
       <c r="F3">
-        <v>0.0308</v>
+        <v>0.4958</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1705,7 +1706,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1714,10 +1715,10 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.0007</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1740,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1749,10 +1750,10 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.0007</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1775,13 +1776,13 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.0308</v>
+        <v>0.4958</v>
       </c>
       <c r="D6">
-        <v>0.0007</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0.0007</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1807,16 +1808,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1866,10 +1867,10 @@
         <v>1</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0.0035</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0.0011</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1901,10 +1902,10 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0.0008</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>0.0046</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1930,16 +1931,16 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0.0035</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0.0008</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1965,13 +1966,408 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0.0011</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0.0046</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.0178</v>
+      </c>
+      <c r="J8">
+        <v>0.1645</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.0178</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.1645</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
       </c>
       <c r="K11">
         <v>1</v>

</xml_diff>